<commit_message>
ok till now in option 4 if i add new cake  then it is adding new quantity and old quantity
</commit_message>
<xml_diff>
--- a/order1.xlsx
+++ b/order1.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,55 +440,173 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CAKE</t>
+          <t>order_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>QUANTITY</t>
+          <t>customer_name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>COST PER CAKE</t>
+          <t>cake</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL COST</t>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cost_per_cake</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>sum_of_each_cake</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>order_date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>rahul</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Classic_Chocolate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
         <v>30</v>
       </c>
-      <c r="D2" t="n">
-        <v>90</v>
+      <c r="F2" t="n">
+        <v>300</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>45282.71052083333</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>rahul</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Vanilla</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
         <v>40</v>
       </c>
-      <c r="D3" t="n">
-        <v>40</v>
+      <c r="F3" t="n">
+        <v>800</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45282.710625</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>raj</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bliss</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1750</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45282.71193287037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>raj</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cookies</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E5" t="n">
+        <v>35</v>
+      </c>
+      <c r="F5" t="n">
+        <v>525</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45282.7121412037</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>rahul</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cookies</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35</v>
+      </c>
+      <c r="F6" t="n">
+        <v>595</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>45282.71256944445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
every thing working fine
</commit_message>
<xml_diff>
--- a/order1.xlsx
+++ b/order1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,16 +489,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>30</v>
       </c>
       <c r="F2" t="n">
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45282.71052083333</v>
+        <v>45283.51190972222</v>
       </c>
     </row>
     <row r="3">
@@ -516,25 +516,25 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
         <v>40</v>
       </c>
       <c r="F3" t="n">
-        <v>800</v>
+        <v>480</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45282.710625</v>
+        <v>45283.51202546297</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>raj</t>
+          <t>rahul</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -543,70 +543,151 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
         <v>35</v>
       </c>
       <c r="F4" t="n">
-        <v>1750</v>
+        <v>350</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45282.71193287037</v>
+        <v>45283.51260416667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>raj</t>
+          <t>rohit</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cookies</t>
+          <t>Red_Velvet</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F5" t="n">
-        <v>525</v>
+        <v>450</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45282.7121412037</v>
+        <v>45283.51989583333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>rahul</t>
+          <t>raj</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Cookies</t>
+          <t>Classic_Chocolate</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" t="n">
+        <v>150</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>45283.52236111111</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>raj</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Bliss</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" t="n">
         <v>35</v>
       </c>
-      <c r="F6" t="n">
-        <v>595</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>45282.71256944445</v>
+      <c r="F7" t="n">
+        <v>280</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>45283.52288194445</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>raj</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Vanilla</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>22</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" t="n">
+        <v>880</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>45283.52310185185</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>raj</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Vanilla</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>55</v>
+      </c>
+      <c r="E9" t="n">
+        <v>40</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2200</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>45283.52400462963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>